<commit_message>
feat: implement YouTube transcript extraction
</commit_message>
<xml_diff>
--- a/data/ohlcv.xlsx
+++ b/data/ohlcv.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,788 +436,1548 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>date</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>open</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>high</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>low</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>close</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>volume</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>value</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>bb_bbm</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>bb_bbh</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>bb_bbl</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>bb_bbhi</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>bb_bbli</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>bb_bbw</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>bb_bbp</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>2025-11-30 09:00</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>20650</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>20980</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>20490</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>20600</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>159342.08477573</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>3302883324.542397</v>
       </c>
+      <c r="I2" t="n">
+        <v>20600</v>
+      </c>
+      <c r="J2" t="n">
+        <v>20600</v>
+      </c>
+      <c r="K2" t="n">
+        <v>20600</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>2025-12-01 09:00</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>20600</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>20640</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>19000</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>19420</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>539767.00571174</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>10525477294.93657</v>
       </c>
+      <c r="I3" t="n">
+        <v>20010</v>
+      </c>
+      <c r="J3" t="n">
+        <v>21190</v>
+      </c>
+      <c r="K3" t="n">
+        <v>18830</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>11.79410294852574</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>2025-12-02 09:00</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>19420</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>20740</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>19210</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>20200</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>312285.89818782</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>6244401518.454654</v>
       </c>
+      <c r="I4" t="n">
+        <v>20073.33333333333</v>
+      </c>
+      <c r="J4" t="n">
+        <v>21053.31065733402</v>
+      </c>
+      <c r="K4" t="n">
+        <v>19093.35600933264</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>9.763972009306118</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.564627345737736</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>2025-12-03 09:00</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>20200</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>21290</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>20090</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>21090</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>313653.21622695</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>6481283966.356035</v>
       </c>
+      <c r="I5" t="n">
+        <v>20327.5</v>
+      </c>
+      <c r="J5" t="n">
+        <v>21550.39615258206</v>
+      </c>
+      <c r="K5" t="n">
+        <v>19104.60384741794</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>12.03193853235331</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.8117599145234183</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>2025-12-04 09:00</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>21090</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>21260</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>20300</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>20500</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>204106.88971305</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>4251363479.472288</v>
       </c>
+      <c r="I6" t="n">
+        <v>20362</v>
+      </c>
+      <c r="J6" t="n">
+        <v>21464.46269778165</v>
+      </c>
+      <c r="K6" t="n">
+        <v>19259.53730221835</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>10.82862879659809</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.5625871516005395</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>2025-12-05 09:00</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>20490</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>20720</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>19450</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>19720</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>247419.09580359</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>4970196705.993962</v>
       </c>
+      <c r="I7" t="n">
+        <v>20186</v>
+      </c>
+      <c r="J7" t="n">
+        <v>21359.00298379842</v>
+      </c>
+      <c r="K7" t="n">
+        <v>19012.99701620158</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>11.62194574257824</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.3013645291459544</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>2025-12-06 09:00</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>19710</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>20130</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>19600</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>19920</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>120088.93458606</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>2381304234.030399</v>
       </c>
+      <c r="I8" t="n">
+        <v>20286</v>
+      </c>
+      <c r="J8" t="n">
+        <v>21246.79966694416</v>
+      </c>
+      <c r="K8" t="n">
+        <v>19325.20033305584</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>9.472539356641589</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.3095336558743454</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>2025-12-07 09:00</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>19940</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>20080</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>19200</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>19630</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>233730.7924919</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>4584855996.080831</v>
       </c>
+      <c r="I9" t="n">
+        <v>20172</v>
+      </c>
+      <c r="J9" t="n">
+        <v>21271.77452234537</v>
+      </c>
+      <c r="K9" t="n">
+        <v>19072.22547765463</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>10.90397107223255</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.2535858537420321</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>2025-12-08 09:00</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>19640</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>20210</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>19540</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>20020</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>163739.22070913</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>3268952197.7349</v>
       </c>
+      <c r="I10" t="n">
+        <v>19958</v>
+      </c>
+      <c r="J10" t="n">
+        <v>20566.78896179218</v>
+      </c>
+      <c r="K10" t="n">
+        <v>19349.21103820782</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>6.100701090211235</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.5509207655617488</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>2025-12-09 09:00</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="C11" t="n">
         <v>20020</v>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>21050</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>19660</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>20540</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>248033.16324054</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>5045286102.816103</v>
       </c>
+      <c r="I11" t="n">
+        <v>19966</v>
+      </c>
+      <c r="J11" t="n">
+        <v>20603.44489957956</v>
+      </c>
+      <c r="K11" t="n">
+        <v>19328.55510042044</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>6.385304012617096</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.9502349931567335</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>2025-12-10 09:00</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="C12" t="n">
         <v>20560</v>
       </c>
-      <c r="C12" t="n">
+      <c r="D12" t="n">
         <v>21110</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>20100</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>20310</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>242819.62334818</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>4964622020.61277</v>
       </c>
+      <c r="I12" t="n">
+        <v>20084</v>
+      </c>
+      <c r="J12" t="n">
+        <v>20713.99682538883</v>
+      </c>
+      <c r="K12" t="n">
+        <v>19454.00317461117</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>6.273619053862071</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.6793659832019904</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>2025-12-11 09:00</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="C13" t="n">
         <v>20320</v>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>20350</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>19380</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>19690</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>295726.16224186</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>5808108555.892374</v>
       </c>
+      <c r="I13" t="n">
+        <v>20038</v>
+      </c>
+      <c r="J13" t="n">
+        <v>20738.78812775332</v>
+      </c>
+      <c r="K13" t="n">
+        <v>19337.21187224668</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>6.994591553581392</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.251708122456594</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>2025-12-12 09:00</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="C14" t="n">
         <v>19700</v>
       </c>
-      <c r="C14" t="n">
+      <c r="D14" t="n">
         <v>19800</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>19020</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>19340</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>240524.24516996</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>4675882645.215843</v>
       </c>
+      <c r="I14" t="n">
+        <v>19980</v>
+      </c>
+      <c r="J14" t="n">
+        <v>20836.87805433445</v>
+      </c>
+      <c r="K14" t="n">
+        <v>19123.12194566555</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>8.577357901245792</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.1265512946897128</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>2025-12-13 09:00</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="C15" t="n">
         <v>19340</v>
       </c>
-      <c r="C15" t="n">
+      <c r="D15" t="n">
         <v>19750</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>19320</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>19670</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>81953.53696574</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>1604937908.417326</v>
       </c>
+      <c r="I15" t="n">
+        <v>19910</v>
+      </c>
+      <c r="J15" t="n">
+        <v>20798.95444202726</v>
+      </c>
+      <c r="K15" t="n">
+        <v>19021.04555797274</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>8.929728197159834</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.3650099551487252</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>2025-12-14 09:00</t>
         </is>
       </c>
-      <c r="B16" t="n">
+      <c r="C16" t="n">
         <v>19660</v>
       </c>
-      <c r="C16" t="n">
+      <c r="D16" t="n">
         <v>19710</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>19000</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>19140</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>150178.5030924</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>2899516595.141441</v>
       </c>
+      <c r="I16" t="n">
+        <v>19630</v>
+      </c>
+      <c r="J16" t="n">
+        <v>20425.88943955804</v>
+      </c>
+      <c r="K16" t="n">
+        <v>18834.11056044196</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>8.108909216077794</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.1921682989837751</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>2025-12-15 09:00</t>
         </is>
       </c>
-      <c r="B17" t="n">
+      <c r="C17" t="n">
         <v>19150</v>
       </c>
-      <c r="C17" t="n">
+      <c r="D17" t="n">
         <v>19640</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>18180</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>18430</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>415825.21918668</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>7865611928.084103</v>
       </c>
+      <c r="I17" t="n">
+        <v>19254</v>
+      </c>
+      <c r="J17" t="n">
+        <v>20175.96312290677</v>
+      </c>
+      <c r="K17" t="n">
+        <v>18332.03687709323</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>9.576847646273681</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.05312746273295015</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>2025-12-16 09:00</t>
         </is>
       </c>
-      <c r="B18" t="n">
+      <c r="C18" t="n">
         <v>18420</v>
       </c>
-      <c r="C18" t="n">
+      <c r="D18" t="n">
         <v>19220</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>18000</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>18870</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>359677.80007934</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>6625596495.075056</v>
       </c>
+      <c r="I18" t="n">
+        <v>19090</v>
+      </c>
+      <c r="J18" t="n">
+        <v>19931.61749031255</v>
+      </c>
+      <c r="K18" t="n">
+        <v>18248.38250968745</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>8.817365011132047</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.3692992941970004</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>2025-12-17 09:00</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="C19" t="n">
         <v>18830</v>
       </c>
-      <c r="C19" t="n">
+      <c r="D19" t="n">
         <v>19000</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>17820</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>18030</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>351338.11720517</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>6452908793.546832</v>
       </c>
+      <c r="I19" t="n">
+        <v>18828</v>
+      </c>
+      <c r="J19" t="n">
+        <v>19960.52991130477</v>
+      </c>
+      <c r="K19" t="n">
+        <v>17695.47008869523</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
+        <v>12.03027311774775</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.1476914242906686</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
         <is>
           <t>2025-12-18 09:00</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="C20" t="n">
         <v>18030</v>
       </c>
-      <c r="C20" t="n">
+      <c r="D20" t="n">
         <v>18460</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>17150</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>17330</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>419451.57199193</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>7467946753.978635</v>
       </c>
+      <c r="I20" t="n">
+        <v>18360</v>
+      </c>
+      <c r="J20" t="n">
+        <v>19638.49912006227</v>
+      </c>
+      <c r="K20" t="n">
+        <v>17081.50087993773</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
+        <v>13.92700566516636</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.09718392299330174</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
         <is>
           <t>2025-12-19 09:00</t>
         </is>
       </c>
-      <c r="B21" t="n">
+      <c r="C21" t="n">
         <v>17330</v>
       </c>
-      <c r="C21" t="n">
+      <c r="D21" t="n">
         <v>18600</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>17150</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>18390</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>335790.93805451</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>6016178587.057446</v>
       </c>
+      <c r="I21" t="n">
+        <v>18210</v>
+      </c>
+      <c r="J21" t="n">
+        <v>19238.86345060946</v>
+      </c>
+      <c r="K21" t="n">
+        <v>17181.13654939054</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
+        <v>11.29998298308025</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0.5874751648984009</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
         <is>
           <t>2025-12-20 09:00</t>
         </is>
       </c>
-      <c r="B22" t="n">
+      <c r="C22" t="n">
         <v>18390</v>
       </c>
-      <c r="C22" t="n">
+      <c r="D22" t="n">
         <v>18780</v>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
         <v>18340</v>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>18420</v>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>144993.68119949</v>
       </c>
-      <c r="G22" t="n">
+      <c r="H22" t="n">
         <v>2679046307.41049</v>
       </c>
+      <c r="I22" t="n">
+        <v>18208</v>
+      </c>
+      <c r="J22" t="n">
+        <v>19235.18255436899</v>
+      </c>
+      <c r="K22" t="n">
+        <v>17180.81744563101</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="n">
+        <v>11.28276092233072</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0.6031948990460777</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
         <is>
           <t>2025-12-21 09:00</t>
         </is>
       </c>
-      <c r="B23" t="n">
+      <c r="C23" t="n">
         <v>18420</v>
       </c>
-      <c r="C23" t="n">
+      <c r="D23" t="n">
         <v>18500</v>
       </c>
-      <c r="D23" t="n">
+      <c r="E23" t="n">
         <v>17900</v>
       </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
         <v>18160</v>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>158906.68646212</v>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>2890328951.831631</v>
       </c>
+      <c r="I23" t="n">
+        <v>18066</v>
+      </c>
+      <c r="J23" t="n">
+        <v>18857.00948161195</v>
+      </c>
+      <c r="K23" t="n">
+        <v>17274.99051838805</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" t="n">
+        <v>8.756885659381661</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0.5594177454159233</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
         <is>
           <t>2025-12-22 09:00</t>
         </is>
       </c>
-      <c r="B24" t="n">
+      <c r="C24" t="n">
         <v>18170</v>
       </c>
-      <c r="C24" t="n">
+      <c r="D24" t="n">
         <v>18580</v>
       </c>
-      <c r="D24" t="n">
+      <c r="E24" t="n">
         <v>18020</v>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
         <v>18290</v>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>143440.45839119</v>
       </c>
-      <c r="G24" t="n">
+      <c r="H24" t="n">
         <v>2629441341.130916</v>
       </c>
+      <c r="I24" t="n">
+        <v>18118</v>
+      </c>
+      <c r="J24" t="n">
+        <v>18926.69277231839</v>
+      </c>
+      <c r="K24" t="n">
+        <v>17309.30722768161</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" t="n">
+        <v>8.926954104408734</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0.60634446472602</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
         <is>
           <t>2025-12-23 09:00</t>
         </is>
       </c>
-      <c r="B25" t="n">
+      <c r="C25" t="n">
         <v>18290</v>
       </c>
-      <c r="C25" t="n">
+      <c r="D25" t="n">
         <v>18380</v>
       </c>
-      <c r="D25" t="n">
+      <c r="E25" t="n">
         <v>17780</v>
       </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
         <v>18030</v>
       </c>
-      <c r="F25" t="n">
+      <c r="G25" t="n">
         <v>122017.70813625</v>
       </c>
-      <c r="G25" t="n">
+      <c r="H25" t="n">
         <v>2201971840.15274</v>
       </c>
+      <c r="I25" t="n">
+        <v>18258</v>
+      </c>
+      <c r="J25" t="n">
+        <v>18549.58875149772</v>
+      </c>
+      <c r="K25" t="n">
+        <v>17966.41124850228</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" t="n">
+        <v>3.194093016734825</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0.109038416556029</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
         <is>
           <t>2025-12-24 09:00</t>
         </is>
       </c>
-      <c r="B26" t="n">
+      <c r="C26" t="n">
         <v>18000</v>
       </c>
-      <c r="C26" t="n">
+      <c r="D26" t="n">
         <v>18030</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
         <v>17460</v>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
         <v>17730</v>
       </c>
-      <c r="F26" t="n">
+      <c r="G26" t="n">
         <v>144994.92851655</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>2559638288.222238</v>
       </c>
+      <c r="I26" t="n">
+        <v>18126</v>
+      </c>
+      <c r="J26" t="n">
+        <v>18599.7256590053</v>
+      </c>
+      <c r="K26" t="n">
+        <v>17652.2743409947</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" t="n">
+        <v>5.22702922879065</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0.08203657277980334</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
         <is>
           <t>2025-12-25 09:00</t>
         </is>
       </c>
-      <c r="B27" t="n">
+      <c r="C27" t="n">
         <v>17730</v>
       </c>
-      <c r="C27" t="n">
+      <c r="D27" t="n">
         <v>17910</v>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="n">
         <v>17210</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>17220</v>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>159103.92001942</v>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>2790345307.03968</v>
       </c>
+      <c r="I27" t="n">
+        <v>17886</v>
+      </c>
+      <c r="J27" t="n">
+        <v>18648.5850772209</v>
+      </c>
+      <c r="K27" t="n">
+        <v>17123.4149227791</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="n">
+        <v>8.527172953381392</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0.06332741100369056</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
         <is>
           <t>2025-12-26 09:00</t>
         </is>
       </c>
-      <c r="B28" t="n">
+      <c r="C28" t="n">
         <v>17210</v>
       </c>
-      <c r="C28" t="n">
+      <c r="D28" t="n">
         <v>17600</v>
       </c>
-      <c r="D28" t="n">
+      <c r="E28" t="n">
         <v>17020</v>
       </c>
-      <c r="E28" t="n">
+      <c r="F28" t="n">
         <v>17190</v>
       </c>
-      <c r="F28" t="n">
+      <c r="G28" t="n">
         <v>252916.10159179</v>
       </c>
-      <c r="G28" t="n">
+      <c r="H28" t="n">
         <v>4364897719.788971</v>
       </c>
+      <c r="I28" t="n">
+        <v>17692</v>
+      </c>
+      <c r="J28" t="n">
+        <v>18562.89838672488</v>
+      </c>
+      <c r="K28" t="n">
+        <v>16821.10161327512</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" t="n">
+        <v>9.845109504011786</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0.2117918647846903</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
         <is>
           <t>2025-12-27 09:00</t>
         </is>
       </c>
-      <c r="B29" t="n">
+      <c r="C29" t="n">
         <v>17190</v>
       </c>
-      <c r="C29" t="n">
+      <c r="D29" t="n">
         <v>17900</v>
       </c>
-      <c r="D29" t="n">
+      <c r="E29" t="n">
         <v>17070</v>
       </c>
-      <c r="E29" t="n">
+      <c r="F29" t="n">
         <v>17840</v>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>166075.18485851</v>
       </c>
-      <c r="G29" t="n">
+      <c r="H29" t="n">
         <v>2881099187.621955</v>
       </c>
+      <c r="I29" t="n">
+        <v>17602</v>
+      </c>
+      <c r="J29" t="n">
+        <v>18278.39041980206</v>
+      </c>
+      <c r="K29" t="n">
+        <v>16925.60958019794</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="n">
+        <v>7.68538143167887</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0.6759338933789524</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
         <is>
           <t>2025-12-28 09:00</t>
         </is>
       </c>
-      <c r="B30" t="n">
+      <c r="C30" t="n">
         <v>17850</v>
       </c>
-      <c r="C30" t="n">
+      <c r="D30" t="n">
         <v>17970</v>
       </c>
-      <c r="D30" t="n">
+      <c r="E30" t="n">
         <v>17530</v>
       </c>
-      <c r="E30" t="n">
+      <c r="F30" t="n">
         <v>17750</v>
       </c>
-      <c r="F30" t="n">
+      <c r="G30" t="n">
         <v>134456.86159791</v>
       </c>
-      <c r="G30" t="n">
+      <c r="H30" t="n">
         <v>2387720618.235114</v>
       </c>
+      <c r="I30" t="n">
+        <v>17546</v>
+      </c>
+      <c r="J30" t="n">
+        <v>18108.08184457426</v>
+      </c>
+      <c r="K30" t="n">
+        <v>16983.91815542574</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="n">
+        <v>6.406951380078181</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0.6814682345366598</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
         <is>
           <t>2025-12-29 09:00</t>
         </is>
       </c>
-      <c r="B31" t="n">
+      <c r="C31" t="n">
         <v>17750</v>
       </c>
-      <c r="C31" t="n">
+      <c r="D31" t="n">
         <v>18060</v>
       </c>
-      <c r="D31" t="n">
-        <v>17500</v>
-      </c>
       <c r="E31" t="n">
-        <v>17670</v>
+        <v>17390</v>
       </c>
       <c r="F31" t="n">
-        <v>130348.28296822</v>
+        <v>17410</v>
       </c>
       <c r="G31" t="n">
-        <v>2327053089.587792</v>
+        <v>149224.44935417</v>
+      </c>
+      <c r="H31" t="n">
+        <v>2657217592.171124</v>
+      </c>
+      <c r="I31" t="n">
+        <v>17482</v>
+      </c>
+      <c r="J31" t="n">
+        <v>18017.97014842247</v>
+      </c>
+      <c r="K31" t="n">
+        <v>16946.02985157753</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" t="n">
+        <v>6.131679995680905</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0.4328320800963271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>